<commit_message>
to #20 new style transfer tests added. Added test gray images
</commit_message>
<xml_diff>
--- a/deepface_project/results.xlsx
+++ b/deepface_project/results.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="results" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="results with ST" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="results gray" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,16 +458,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6567164179104478</v>
+        <v>0.5925925925925926</v>
       </c>
       <c r="C2" t="n">
-        <v>0.65625</v>
+        <v>0.6</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6461538461538462</v>
+        <v>0.576923076923077</v>
       </c>
     </row>
     <row r="3">
@@ -476,16 +477,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5373134328358209</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="C3" t="n">
-        <v>0.53125</v>
+        <v>0.6521739130434783</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5151515151515151</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5230769230769231</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4">
@@ -495,16 +496,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.746268656716418</v>
+        <v>0.5185185185185185</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6904761904761905</v>
+        <v>0.5238095238095238</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8787878787878788</v>
+        <v>0.4074074074074074</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7733333333333333</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="5">
@@ -514,16 +515,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5074626865671642</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5</v>
+        <v>0.4482758620689655</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.4814814814814815</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.4642857142857143</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +534,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5</v>
+        <v>0.4516129032258064</v>
       </c>
       <c r="D6" t="n">
-        <v>0.303030303030303</v>
+        <v>0.5185185185185185</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3773584905660378</v>
+        <v>0.4827586206896551</v>
       </c>
     </row>
     <row r="7">
@@ -552,16 +553,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5757575757575758</v>
+        <v>0.462962962962963</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5471698113207547</v>
+        <v>0.46875</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8787878787878788</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6744186046511628</v>
+        <v>0.5084745762711864</v>
       </c>
     </row>
     <row r="8">
@@ -571,16 +572,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4776119402985075</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="D8" t="n">
-        <v>0.696969696969697</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5679012345679013</v>
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>
@@ -636,16 +637,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7164179104477612</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7164179104477613</v>
+        <v>0.6296296296296297</v>
       </c>
     </row>
     <row r="3">
@@ -655,16 +656,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.746268656716418</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="C3" t="n">
-        <v>0.75</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.5925925925925926</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7384615384615384</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="4">
@@ -674,16 +675,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7313432835820896</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6829268292682927</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8484848484848485</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7567567567567567</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="5">
@@ -693,16 +694,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5671641791044776</v>
+        <v>0.5185185185185185</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5625</v>
+        <v>0.52</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.4814814814814815</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5538461538461538</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
@@ -712,16 +713,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5151515151515151</v>
+        <v>0.4259259259259259</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.4230769230769231</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2424242424242424</v>
+        <v>0.4074074074074074</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.4150943396226415</v>
       </c>
     </row>
     <row r="7">
@@ -731,16 +732,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5909090909090909</v>
+        <v>0.462962962962963</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5535714285714286</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9393939393939394</v>
+        <v>0.5185185185185185</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6966292134831461</v>
+        <v>0.4912280701754386</v>
       </c>
     </row>
     <row r="8">
@@ -750,16 +751,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5522388059701493</v>
+        <v>0.5</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5348837209302325</v>
+        <v>0.5</v>
       </c>
       <c r="D8" t="n">
-        <v>0.696969696969697</v>
+        <v>0.7037037037037037</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6052631578947368</v>
+        <v>0.5846153846153846</v>
       </c>
     </row>
   </sheetData>
@@ -768,6 +769,185 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>backbone</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>precision</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>recall</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>VGG-Face</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.6851851851851852</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.6470588235294118</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.8148148148148148</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7213114754098361</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Facenet</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5925925925925926</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.576923076923077</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Facenet512</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.6111111111111112</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3703703703703703</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.4878048780487805</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>OpenFace</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5384615384615384</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6363636363636364</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DeepFace</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4259259259259259</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5185185185185185</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.4745762711864406</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DeepID</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.4814814814814815</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.4871794871794872</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.7037037037037037</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.5757575757575758</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ArcFace</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.4814814814814815</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.4761904761904762</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.3703703703703703</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.4166666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>